<commit_message>
Complete mobile data retrieved. Limited data set to SE Asia 11 countries.
</commit_message>
<xml_diff>
--- a/Data/City Data.xlsx
+++ b/Data/City Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaretpearce/Documents/Graduate Coursework/LIS 677/Project/Raw data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaretpearce/Documents/Graduate Coursework/LIS 677/Project/lis677-project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="1520" windowWidth="28160" windowHeight="15420" tabRatio="500"/>
+    <workbookView xWindow="12700" yWindow="460" windowWidth="15360" windowHeight="15980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Capitals" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Country</t>
   </si>
   <si>
-    <t>Bangladesh</t>
-  </si>
-  <si>
     <t>Brunei Darussalam</t>
   </si>
   <si>
@@ -41,27 +38,15 @@
     <t>Indonesia</t>
   </si>
   <si>
-    <t>Iraq</t>
-  </si>
-  <si>
     <t>Lao PDR</t>
   </si>
   <si>
     <t>Malaysia</t>
   </si>
   <si>
-    <t>Maldives</t>
-  </si>
-  <si>
-    <t>Mongolia</t>
-  </si>
-  <si>
     <t>Myanmar</t>
   </si>
   <si>
-    <t>Pakistan</t>
-  </si>
-  <si>
     <t>Philippines</t>
   </si>
   <si>
@@ -74,9 +59,6 @@
     <t>Timor-Leste</t>
   </si>
   <si>
-    <t>Vanuatu</t>
-  </si>
-  <si>
     <t>Vietnam</t>
   </si>
   <si>
@@ -89,9 +71,6 @@
     <t>Longitude</t>
   </si>
   <si>
-    <t>Dhaka</t>
-  </si>
-  <si>
     <t>Bandar Seri Begawan</t>
   </si>
   <si>
@@ -101,27 +80,15 @@
     <t>Jakarta</t>
   </si>
   <si>
-    <t>Baghdad</t>
-  </si>
-  <si>
     <t>Vientiane</t>
   </si>
   <si>
     <t>Kuala Lumpur</t>
   </si>
   <si>
-    <t>Ulaanbaatar</t>
-  </si>
-  <si>
-    <t>Malé</t>
-  </si>
-  <si>
     <t>Naypyidaw</t>
   </si>
   <si>
-    <t>Islamabad</t>
-  </si>
-  <si>
     <t>Manila</t>
   </si>
   <si>
@@ -129,9 +96,6 @@
   </si>
   <si>
     <t>Dili</t>
-  </si>
-  <si>
-    <t>Port Vila</t>
   </si>
   <si>
     <t>Hanoi</t>
@@ -154,7 +118,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -195,7 +159,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,25 +459,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -521,28 +485,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2">
-        <v>23.7805733</v>
+        <v>4.9061376000000001</v>
       </c>
       <c r="D2" s="2">
-        <v>90.279238899999996</v>
+        <v>114.8680495</v>
       </c>
       <c r="E2">
-        <v>315</v>
+        <v>38.75</v>
       </c>
       <c r="F2">
-        <f>E2*2.58999</f>
-        <v>815.8468499999999</v>
+        <f t="shared" ref="F2:F12" si="0">E2*2.58999</f>
+        <v>100.36211249999999</v>
       </c>
       <c r="G2">
-        <f>SQRT(F2)</f>
-        <v>28.563032927194548</v>
+        <f t="shared" ref="G2:G12" si="1">SQRT(F2)</f>
+        <v>10.01808926392653</v>
       </c>
       <c r="H2">
-        <f>_xlfn.CEILING.MATH(G2)</f>
-        <v>29</v>
+        <f t="shared" ref="H2:H12" si="2">_xlfn.CEILING.MATH(G2)</f>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -550,28 +514,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2">
-        <v>4.9061376000000001</v>
+        <v>11.5793306</v>
       </c>
       <c r="D3" s="2">
-        <v>114.8680495</v>
+        <v>104.7500991</v>
       </c>
       <c r="E3">
-        <v>38.75</v>
+        <v>262</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F18" si="0">E3*2.58999</f>
-        <v>100.36211249999999</v>
+        <f t="shared" si="0"/>
+        <v>678.57737999999995</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G18" si="1">SQRT(F3)</f>
-        <v>10.01808926392653</v>
+        <f t="shared" si="1"/>
+        <v>26.049517845825861</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H18" si="2">_xlfn.CEILING.MATH(G3)</f>
-        <v>11</v>
+        <f t="shared" si="2"/>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -579,28 +543,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2">
-        <v>11.5793306</v>
+        <v>-6.2297279999999997</v>
       </c>
       <c r="D4" s="2">
-        <v>104.7500991</v>
+        <v>106.6894301</v>
       </c>
       <c r="E4">
-        <v>262</v>
+        <v>256.39999999999998</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>678.57737999999995</v>
+        <v>664.0734359999999</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
-        <v>26.049517845825861</v>
+        <v>25.769622348804415</v>
       </c>
       <c r="H4">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -608,28 +572,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2">
-        <v>-6.2297279999999997</v>
+        <v>17.960426999999999</v>
       </c>
       <c r="D5" s="2">
-        <v>106.6894301</v>
+        <v>102.53572490000001</v>
       </c>
       <c r="E5">
-        <v>256.39999999999998</v>
+        <v>1514</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>664.0734359999999</v>
+        <v>3921.2448599999998</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
-        <v>25.769622348804415</v>
+        <v>62.61984397936488</v>
       </c>
       <c r="H5">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -637,28 +601,28 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2">
-        <v>33.311607500000001</v>
+        <v>3.1390006000000001</v>
       </c>
       <c r="D6" s="2">
-        <v>44.215819199999999</v>
+        <v>101.6168146</v>
       </c>
       <c r="E6">
-        <v>78.84</v>
+        <v>93.82</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>204.19481159999998</v>
+        <v>242.99286179999996</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
-        <v>14.289674999803179</v>
+        <v>15.588228308566691</v>
       </c>
       <c r="H6">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -666,28 +630,28 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2">
-        <v>17.960426999999999</v>
+        <v>19.746996299999999</v>
       </c>
       <c r="D7" s="2">
-        <v>102.53572490000001</v>
+        <v>96.053389499999994</v>
       </c>
       <c r="E7">
-        <v>1514</v>
+        <v>2724</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>3921.2448599999998</v>
+        <v>7055.1327599999995</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
-        <v>62.61984397936488</v>
+        <v>83.994837698515738</v>
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -695,28 +659,28 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2">
-        <v>3.1390006000000001</v>
+        <v>14.598068899999999</v>
       </c>
       <c r="D8" s="2">
-        <v>101.6168146</v>
+        <v>120.94463159999999</v>
       </c>
       <c r="E8">
-        <v>93.82</v>
+        <v>14.88</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>242.99286179999996</v>
+        <v>38.539051199999996</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
-        <v>15.588228308566691</v>
+        <v>6.2079828608010832</v>
       </c>
       <c r="H8">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -724,28 +688,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2">
-        <v>4.1770898000000001</v>
+        <v>1.3147150000000001</v>
       </c>
       <c r="D9" s="2">
-        <v>73.501257699999996</v>
+        <v>103.5668182</v>
       </c>
       <c r="E9">
-        <v>2.2389999999999999</v>
+        <v>277.60000000000002</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>5.7989876099999993</v>
+        <v>718.981224</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
-        <v>2.4081087205522924</v>
+        <v>26.813825239976484</v>
       </c>
       <c r="H9">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -753,28 +717,28 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2">
-        <v>47.891564899999999</v>
+        <v>13.7244426</v>
       </c>
       <c r="D10" s="2">
-        <v>106.76178760000001</v>
+        <v>100.3529114</v>
       </c>
       <c r="E10">
-        <v>1816.3</v>
+        <v>606</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>4704.1988369999999</v>
+        <v>1569.5339399999998</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>68.587162333777883</v>
+        <v>39.617343929142947</v>
       </c>
       <c r="H10">
         <f t="shared" si="2"/>
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -782,28 +746,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C11" s="2">
-        <v>19.746996299999999</v>
+        <v>-8.5564496999999999</v>
       </c>
       <c r="D11" s="2">
-        <v>96.053389499999994</v>
+        <v>125.4999306</v>
       </c>
       <c r="E11">
-        <v>2724</v>
+        <v>18.64</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>7055.1327599999995</v>
+        <v>48.277413599999996</v>
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
-        <v>83.994837698515738</v>
+        <v>6.948194988628341</v>
       </c>
       <c r="H11">
         <f t="shared" si="2"/>
-        <v>84</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -811,200 +775,26 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C12" s="2">
-        <v>33.669055499999999</v>
+        <v>21.022693100000001</v>
       </c>
       <c r="D12" s="2">
-        <v>72.844891500000003</v>
+        <v>105.8019441</v>
       </c>
       <c r="E12">
-        <v>349.8</v>
+        <v>1291</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>905.97850199999993</v>
+        <v>3343.6770899999997</v>
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
-        <v>30.099476772861017</v>
+        <v>57.824537092829367</v>
       </c>
       <c r="H12">
-        <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="2">
-        <v>14.598068899999999</v>
-      </c>
-      <c r="D13" s="2">
-        <v>120.94463159999999</v>
-      </c>
-      <c r="E13">
-        <v>14.88</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>38.539051199999996</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="1"/>
-        <v>6.2079828608010832</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1.3147150000000001</v>
-      </c>
-      <c r="D14" s="2">
-        <v>103.5668182</v>
-      </c>
-      <c r="E14">
-        <v>277.60000000000002</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>718.981224</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="1"/>
-        <v>26.813825239976484</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="2">
-        <v>13.7244426</v>
-      </c>
-      <c r="D15" s="2">
-        <v>100.3529114</v>
-      </c>
-      <c r="E15">
-        <v>606</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>1569.5339399999998</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="1"/>
-        <v>39.617343929142947</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="2">
-        <v>-8.5564496999999999</v>
-      </c>
-      <c r="D16" s="2">
-        <v>125.4999306</v>
-      </c>
-      <c r="E16">
-        <v>18.64</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>48.277413599999996</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="1"/>
-        <v>6.948194988628341</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="2">
-        <v>-17.736940199999999</v>
-      </c>
-      <c r="D17" s="2">
-        <v>168.28779449999999</v>
-      </c>
-      <c r="E17">
-        <v>2.073369</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>5.3700049763099997</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="1"/>
-        <v>2.31732711896918</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="2">
-        <v>21.022693100000001</v>
-      </c>
-      <c r="D18" s="2">
-        <v>105.8019441</v>
-      </c>
-      <c r="E18">
-        <v>1291</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="0"/>
-        <v>3343.6770899999997</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="1"/>
-        <v>57.824537092829367</v>
-      </c>
-      <c r="H18">
         <f t="shared" si="2"/>
         <v>58</v>
       </c>

</xml_diff>